<commit_message>
Fix example config format - use LevelNames column
The config loader expects:
- LevelNames column with comma-separated values
- NOT Level1, Level2, Level3 separate columns

Corrected example_config.xlsx to use proper format:
- AttributeName, AttributeLabel, NumLevels, LevelNames

Example:
  Brand | Brand | 4 | Apple, Samsung, Google, OnePlus
</commit_message>
<xml_diff>
--- a/modules/conjoint/examples/example_config.xlsx
+++ b/modules/conjoint/examples/example_config.xlsx
@@ -725,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -737,12 +737,7 @@
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -763,32 +758,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Level1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Level2</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Level3</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Level4</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Level5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Level6</t>
+          <t>LevelNames</t>
         </is>
       </c>
     </row>
@@ -808,22 +778,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apple</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>OnePlus</t>
+          <t>Apple, Samsung, Google, OnePlus</t>
         </is>
       </c>
     </row>
@@ -843,22 +798,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$299</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>$399</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>$499</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>$599</t>
+          <t>$299, $399, $499, $599</t>
         </is>
       </c>
     </row>
@@ -878,17 +818,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.5 inches</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6.1 inches</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>6.7 inches</t>
+          <t>5.5 inches, 6.1 inches, 6.7 inches</t>
         </is>
       </c>
     </row>
@@ -908,17 +838,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12 hours</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>18 hours</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>24 hours</t>
+          <t>12 hours, 18 hours, 24 hours</t>
         </is>
       </c>
     </row>
@@ -938,17 +858,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Basic</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Excellent</t>
+          <t>Basic, Good, Excellent</t>
         </is>
       </c>
     </row>
@@ -963,7 +873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,7 +891,9 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -989,7 +901,9 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -1025,7 +939,9 @@
         </is>
       </c>
     </row>
-    <row r="10"/>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
@@ -1068,7 +984,9 @@
         </is>
       </c>
     </row>
-    <row r="17"/>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
@@ -1104,7 +1022,9 @@
         </is>
       </c>
     </row>
-    <row r="23"/>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
@@ -1122,20 +1042,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>- Adjust settings in the Settings sheet</t>
+          <t>- LevelNames should be comma-separated (e.g., 'Level1, Level2, Level3')</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>- Adjust settings in the Settings sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>- Update data_file path to point to your data</t>
         </is>
       </c>
     </row>
-    <row r="28"/>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>For more information, see the specification documents in modules/conjoint/</t>
         </is>

</xml_diff>

<commit_message>
Fix config file paths - remove duplicate examples/ prefix
- Changed data_file from 'examples/sample_cbc_data.csv' to 'sample_cbc_data.csv'
- Changed output_file from 'examples/output/...' to 'output/...'
- Paths are now correctly relative to config file location
- Fixes double 'examples/examples' path issue
</commit_message>
<xml_diff>
--- a/modules/conjoint/examples/example_config.xlsx
+++ b/modules/conjoint/examples/example_config.xlsx
@@ -569,7 +569,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>examples/sample_cbc_data.csv</t>
+          <t>sample_cbc_data.csv</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>examples/output/example_results.xlsx</t>
+          <t>output/example_results.xlsx</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -891,9 +891,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -901,9 +899,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -939,9 +935,7 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-    </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
@@ -984,9 +978,7 @@
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-    </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
@@ -1022,9 +1014,7 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-    </row>
+    <row r="23"/>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
@@ -1060,9 +1050,7 @@
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr"/>
-    </row>
+    <row r="29"/>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>

</xml_diff>